<commit_message>
Tianlun Li diary 1/16 (#64)
* Tianlun Li diary 1/16
</commit_message>
<xml_diff>
--- a/diaries/diary-Tianlun Li.xlsx
+++ b/diaries/diary-Tianlun Li.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/litianlun/Winter2020/265/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7702CB90-32D8-3346-BE3B-2216A2EFC293}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{154C3F45-902A-4145-A047-757CF6423648}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32800" yWindow="2720" windowWidth="28060" windowHeight="17540" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="-32800" yWindow="2720" windowWidth="31920" windowHeight="17540" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Achievements</t>
   </si>
   <si>
-    <t>Etc.</t>
-  </si>
-  <si>
     <t>Tianlun Li</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
@@ -97,6 +94,46 @@
   </si>
   <si>
     <t>Looking forward to dive deeper</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>5:00 - 8:05 p.m.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Learn the basic strategies of  understanding source codes</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Read and debuged the pacman project, listened to google alumni talking about engineering and management in google</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>We do not need to understand the whole project to debug. Only read the necessary code. Working at google is soooo coooool</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pretty Good</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>7:00 - 8:00 p.m.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Build the Jedit project and find one more project to build</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Successfully built the Jedit project , downloaded a project called jadx and built the project following the readme.md</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>If there's a readme along with the project, your life would be much easier</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Happy</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
@@ -243,7 +280,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -269,19 +306,22 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="14" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="差" xfId="2" builtinId="27"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="4" builtinId="8"/>
-    <cellStyle name="好" xfId="1" builtinId="26"/>
-    <cellStyle name="适中" xfId="3" builtinId="28"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -297,7 +337,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -593,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
-  <dimension ref="A1:G125"/>
+  <dimension ref="A1:G126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -605,24 +645,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7" ht="16">
       <c r="A3" s="1"/>
@@ -638,7 +678,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -650,8 +690,8 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>12</v>
+      <c r="B5" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -663,8 +703,8 @@
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>13</v>
+      <c r="B6" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -707,7 +747,7 @@
         <v>9</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>7</v>
@@ -715,47 +755,69 @@
     </row>
     <row r="10" spans="1:7" ht="34">
       <c r="A10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>15</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="G10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="8" t="s">
+    </row>
+    <row r="11" spans="1:7" ht="68">
+      <c r="A11" s="11">
+        <v>43840</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="68">
+      <c r="A12" s="11">
+        <v>43846</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="16">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:7" ht="16">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
       <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="1:7" ht="17">
-      <c r="A13" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="D12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="16">
+      <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -791,19 +853,19 @@
       <c r="G16" s="8"/>
     </row>
     <row r="17" spans="1:7" ht="16">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:7" ht="16">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="6"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="8"/>
@@ -812,7 +874,7 @@
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
-      <c r="D19" s="8"/>
+      <c r="D19" s="6"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="8"/>
@@ -839,7 +901,7 @@
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
+      <c r="D22" s="8"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="8"/>
@@ -1770,6 +1832,15 @@
       <c r="E125" s="7"/>
       <c r="F125" s="7"/>
       <c r="G125" s="8"/>
+    </row>
+    <row r="126" spans="1:7" ht="16">
+      <c r="A126" s="7"/>
+      <c r="B126" s="7"/>
+      <c r="C126" s="7"/>
+      <c r="D126" s="7"/>
+      <c r="E126" s="7"/>
+      <c r="F126" s="7"/>
+      <c r="G126" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
tianlun diary 1.26 update
</commit_message>
<xml_diff>
--- a/diaries/diary-Tianlun Li.xlsx
+++ b/diaries/diary-Tianlun Li.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/litianlun/Winter2020/265/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{154C3F45-902A-4145-A047-757CF6423648}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC34E29-5585-4449-83D8-D971F3AAEF9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32800" yWindow="2720" windowWidth="31920" windowHeight="17540" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -134,6 +134,42 @@
   </si>
   <si>
     <t>Happy</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>2:00 - 3:30 p.m.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finish the pacman homework</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished the pacman hw</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>PacMan is not a big app, but we still need to take some time reading the code. Fortunately we don't need to read every line of  code to make modification to the application</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cool</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Learn about mental models, how to externalize mental model and  how to model the code using UML graph</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Worried, because the homework sounds intimidating</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Explored the pacman features by locating the code that implemented the feature. Built the UML graph of pacman using intellij plugin</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mental model exist in our daily life. Learning how to externalize it is important for software engineers to commnuicate their ideas with other people</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
@@ -309,11 +345,11 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -636,7 +672,7 @@
   <dimension ref="A1:G126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -645,24 +681,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:7" ht="16">
       <c r="A3" s="1"/>
@@ -775,7 +811,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="68">
-      <c r="A11" s="11">
+      <c r="A11" s="10">
         <v>43840</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -796,7 +832,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="68">
-      <c r="A12" s="11">
+      <c r="A12" s="10">
         <v>43846</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -816,23 +852,47 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="16">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
+    <row r="13" spans="1:7" ht="85">
+      <c r="A13" s="10">
+        <v>43849</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:7" ht="16">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
+      <c r="D13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="85">
+      <c r="A14" s="10">
+        <v>43853</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="8"/>
+      <c r="D14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="16">
       <c r="A15" s="7"/>

</xml_diff>

<commit_message>
tianlun diary 1.29 update
</commit_message>
<xml_diff>
--- a/diaries/diary-Tianlun Li.xlsx
+++ b/diaries/diary-Tianlun Li.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/litianlun/Winter2020/265/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AB6548-A3F8-244B-A2D0-BAB1E63EEA24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E39D3AE-8238-624D-BBB0-DA459F217122}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -170,6 +170,50 @@
   </si>
   <si>
     <t>Mental model exist in our daily life. Learning how to externalize it is important for software engineers to commnuicate their ideas with other people</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>9/00 - 12:00 p.m.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zeyu Huang, Yue Zhang</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Export uml graph</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>2:00 - 5:00 p.m.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Learn about the features of elasticsearch and decide which two features we want to dive in</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">We choose ip filtering and rank evaluation </t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Confused </t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Elasticsearch is an incredible project with tons of great features. It seems pretty intimidating at first glance</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>The project has very loose coupling, so we don't relly need the uml graph for the whole project, just the parts we need</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Elasticsearch is too big to draw an uml graph, with over 10k java classes, the graph is impossible to print out, so we took the parts we looked into and drawed some smaller uml graph</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Good</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
@@ -672,7 +716,7 @@
   <dimension ref="A1:G126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:G14"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -894,23 +938,51 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="16">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="1:7" ht="16">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="8"/>
+    <row r="15" spans="1:7" ht="51">
+      <c r="A15" s="10">
+        <v>43855</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="85">
+      <c r="A16" s="10">
+        <v>43859</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="16">
       <c r="A17" s="7"/>

</xml_diff>

<commit_message>
tianlun diary 1.30-2.5 (#262)
</commit_message>
<xml_diff>
--- a/diaries/diary-Tianlun Li.xlsx
+++ b/diaries/diary-Tianlun Li.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/litianlun/Winter2020/265/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E39D3AE-8238-624D-BBB0-DA459F217122}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A48F3A-68CF-1547-BF89-35B65CD442AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="68">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -214,6 +214,78 @@
   </si>
   <si>
     <t>Good</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>7:00-9:00p.m.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>1:00-5:00 p.m.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>9/00 - 11:30p.m.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Learn about structural and behavioral model; Learn UML diagram and other diagrams. Talk with the alumni from Argentina</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>We learned about KEP, structural and behavior model, and different kinds of diagrams</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>I am still a little confused about those diagrams, what are the use cases of the diagrams.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Relaxed</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get elasticsearch up and running on our computer, try out some features of elasticsearch</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get elasticsearch running on my computer,tried index some documents and then search them</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Elasticsearch is an powerful yet complex tool, we only touched a small part of it</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Excited</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Try to understand the index and search functionalities</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>The system is very loose coupled and reflected some architecture such as public and subscribe we learned on the other course. But it makes it very hard to trace the functionality.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Read the source code of indexing and searching but didn't fully understand.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished!</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finish the homework. We are planning write reports, draw some graphs ourselves.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished the homework but not very confident to our work.</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>gooood</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
@@ -360,7 +432,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -394,6 +466,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -715,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -984,41 +1059,95 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="16">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
+    <row r="17" spans="1:7" ht="68">
+      <c r="A17" s="10">
+        <v>43860</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>14</v>
+      </c>
       <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="1:7" ht="16">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="1:7" ht="16">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="8"/>
-    </row>
-    <row r="20" spans="1:7" ht="16">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="8"/>
+      <c r="D17" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="51">
+      <c r="A18" s="10">
+        <v>43861</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="85">
+      <c r="A19" s="10">
+        <v>43864</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="34">
+      <c r="A20" s="10">
+        <v>43866</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="16">
       <c r="A21" s="7"/>

</xml_diff>